<commit_message>
mainActiviter lit/recupére les donné excel + sur excel rajoue calcule
dans le fichier excel dans la cologne 1 j'ai rajouter un calcule de somme pour eviter de parcourir tout la feuille sur android
</commit_message>
<xml_diff>
--- a/main/assets/finance.xlsx
+++ b/main/assets/finance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18500" windowHeight="11020" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18500" windowHeight="11020" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="eparne" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,96 +396,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B2">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B4">
-        <v>5.9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -495,33 +406,32 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <f ca="1">OFFSET(B1,COUNTA(B:B)-1,)</f>
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+      <c r="E1">
+        <f>SUM(C2:C1000)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>46023</v>
       </c>
-      <c r="B2" s="1">
-        <v>46023</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -530,49 +440,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B2">
-        <v>1500</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -582,27 +452,196 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <f>SUM(B2:B1000)</f>
+        <v>34.9</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>46023</v>
       </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>46023</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>46023</v>
+      </c>
+      <c r="B4">
+        <v>5.9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <f ca="1">SUMIFS(C:C,A:A, "&lt;="&amp;TODAY(),B:B, "&gt;"&amp;TODAY())</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>46023</v>
+      </c>
       <c r="B2" s="1">
+        <v>46054</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <f>SUM(B2:B1000)</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
         <v>46023</v>
+      </c>
+      <c r="B2">
+        <v>1500</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <f ca="1">SUMIFS(C:C,A:A, "&lt;="&amp;TODAY(),B:B, "&gt;"&amp;TODAY())</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>46023</v>
+      </c>
+      <c r="B2" s="1">
+        <v>46054</v>
       </c>
       <c r="C2">
         <v>2000</v>
@@ -610,6 +649,9 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rajoue de add eparne est des gain et depence
bug sur depence courant qui affiche les depence continue alors que j'uttilise la bonne feuille de lecture
bug sur les calcule de gain et donc dans le calcule de l'eparne
mais si on mais a jour tout se remet a jour sinon
</commit_message>
<xml_diff>
--- a/main/assets/finance.xlsx
+++ b/main/assets/finance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18500" windowHeight="11020" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18500" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="eparne" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>date_debut</t>
   </si>
@@ -45,24 +45,6 @@
   </si>
   <si>
     <t>descritpion</t>
-  </si>
-  <si>
-    <t>cours</t>
-  </si>
-  <si>
-    <t>netflix</t>
-  </si>
-  <si>
-    <t>salaire</t>
-  </si>
-  <si>
-    <t>prime</t>
-  </si>
-  <si>
-    <t>Crunchyrol</t>
-  </si>
-  <si>
-    <t>ADN</t>
   </si>
 </sst>
 </file>
@@ -398,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -445,7 +427,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -465,41 +447,17 @@
       </c>
       <c r="E1">
         <f>SUM(B2:B1000)</f>
-        <v>34.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B2">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B4">
-        <v>5.9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -512,7 +470,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -535,22 +493,12 @@
       </c>
       <c r="F1">
         <f ca="1">SUMIFS(C:C,A:A, "&lt;="&amp;TODAY(),B:B, "&gt;"&amp;TODAY())</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B2" s="1">
-        <v>46054</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="2"/>
@@ -566,7 +514,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -586,19 +534,11 @@
       </c>
       <c r="E1">
         <f>SUM(B2:B1000)</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B2">
-        <v>1500</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -609,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -633,22 +573,12 @@
       </c>
       <c r="F1">
         <f ca="1">SUMIFS(C:C,A:A, "&lt;="&amp;TODAY(),B:B, "&gt;"&amp;TODAY())</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>46023</v>
-      </c>
-      <c r="B2" s="1">
-        <v>46054</v>
-      </c>
-      <c r="C2">
-        <v>2000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="1"/>

</xml_diff>